<commit_message>
Work 3 finished :)
</commit_message>
<xml_diff>
--- a/Trabajo_3/Normalized_data.xlsx
+++ b/Trabajo_3/Normalized_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F304"/>
+  <dimension ref="A1:D304"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,16 +454,6 @@
           <t>thalachh</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>oldpeak</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>thall</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -478,12 +468,6 @@
       <c r="D2" t="n">
         <v>0.6030534351145038</v>
       </c>
-      <c r="E2" t="n">
-        <v>0.3709677419354838</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -498,12 +482,6 @@
       <c r="D3" t="n">
         <v>0.8854961832061069</v>
       </c>
-      <c r="E3" t="n">
-        <v>0.564516129032258</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -518,12 +496,6 @@
       <c r="D4" t="n">
         <v>0.7709923664122137</v>
       </c>
-      <c r="E4" t="n">
-        <v>0.2258064516129032</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -538,12 +510,6 @@
       <c r="D5" t="n">
         <v>0.816793893129771</v>
       </c>
-      <c r="E5" t="n">
-        <v>0.1290322580645161</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -558,12 +524,6 @@
       <c r="D6" t="n">
         <v>0.7022900763358778</v>
       </c>
-      <c r="E6" t="n">
-        <v>0.09677419354838709</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -578,12 +538,6 @@
       <c r="D7" t="n">
         <v>0.5877862595419847</v>
       </c>
-      <c r="E7" t="n">
-        <v>0.06451612903225806</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -598,12 +552,6 @@
       <c r="D8" t="n">
         <v>0.6259541984732825</v>
       </c>
-      <c r="E8" t="n">
-        <v>0.2096774193548387</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -618,12 +566,6 @@
       <c r="D9" t="n">
         <v>0.7786259541984732</v>
       </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -638,12 +580,6 @@
       <c r="D10" t="n">
         <v>0.6946564885496184</v>
       </c>
-      <c r="E10" t="n">
-        <v>0.08064516129032258</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -658,12 +594,6 @@
       <c r="D11" t="n">
         <v>0.7862595419847328</v>
       </c>
-      <c r="E11" t="n">
-        <v>0.2580645161290323</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -678,12 +608,6 @@
       <c r="D12" t="n">
         <v>0.6793893129770993</v>
       </c>
-      <c r="E12" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -698,12 +622,6 @@
       <c r="D13" t="n">
         <v>0.5190839694656488</v>
       </c>
-      <c r="E13" t="n">
-        <v>0.03225806451612903</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -718,12 +636,6 @@
       <c r="D14" t="n">
         <v>0.7633587786259542</v>
       </c>
-      <c r="E14" t="n">
-        <v>0.09677419354838709</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -738,12 +650,6 @@
       <c r="D15" t="n">
         <v>0.5572519083969466</v>
       </c>
-      <c r="E15" t="n">
-        <v>0.2903225806451613</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -758,12 +664,6 @@
       <c r="D16" t="n">
         <v>0.6946564885496184</v>
       </c>
-      <c r="E16" t="n">
-        <v>0.1612903225806452</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -778,12 +678,6 @@
       <c r="D17" t="n">
         <v>0.6641221374045801</v>
       </c>
-      <c r="E17" t="n">
-        <v>0.2580645161290323</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -798,12 +692,6 @@
       <c r="D18" t="n">
         <v>0.7709923664122137</v>
       </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -818,12 +706,6 @@
       <c r="D19" t="n">
         <v>0.3282442748091603</v>
       </c>
-      <c r="E19" t="n">
-        <v>0.4193548387096774</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -838,12 +720,6 @@
       <c r="D20" t="n">
         <v>0.7633587786259542</v>
       </c>
-      <c r="E20" t="n">
-        <v>0.2419354838709677</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -858,12 +734,6 @@
       <c r="D21" t="n">
         <v>0.6106870229007634</v>
       </c>
-      <c r="E21" t="n">
-        <v>0.2903225806451613</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -878,12 +748,6 @@
       <c r="D22" t="n">
         <v>0.6870229007633588</v>
       </c>
-      <c r="E22" t="n">
-        <v>0.08064516129032258</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -898,12 +762,6 @@
       <c r="D23" t="n">
         <v>0.8244274809160306</v>
       </c>
-      <c r="E23" t="n">
-        <v>0.06451612903225806</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -918,12 +776,6 @@
       <c r="D24" t="n">
         <v>0.816793893129771</v>
       </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -938,12 +790,6 @@
       <c r="D25" t="n">
         <v>0.5038167938931297</v>
       </c>
-      <c r="E25" t="n">
-        <v>0.1612903225806452</v>
-      </c>
-      <c r="F25" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -958,12 +804,6 @@
       <c r="D26" t="n">
         <v>0.816793893129771</v>
       </c>
-      <c r="E26" t="n">
-        <v>0.2258064516129032</v>
-      </c>
-      <c r="F26" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -978,12 +818,6 @@
       <c r="D27" t="n">
         <v>0.6946564885496184</v>
       </c>
-      <c r="E27" t="n">
-        <v>0.06451612903225806</v>
-      </c>
-      <c r="F27" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -998,12 +832,6 @@
       <c r="D28" t="n">
         <v>0.6564885496183206</v>
       </c>
-      <c r="E28" t="n">
-        <v>0.2580645161290323</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1018,12 +846,6 @@
       <c r="D29" t="n">
         <v>0.3969465648854962</v>
       </c>
-      <c r="E29" t="n">
-        <v>0.09677419354838709</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1038,12 +860,6 @@
       <c r="D30" t="n">
         <v>0.6564885496183206</v>
       </c>
-      <c r="E30" t="n">
-        <v>0.1290322580645161</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1058,12 +874,6 @@
       <c r="D31" t="n">
         <v>0.6183206106870229</v>
       </c>
-      <c r="E31" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F31" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1078,12 +888,6 @@
       <c r="D32" t="n">
         <v>0.7404580152671756</v>
       </c>
-      <c r="E32" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1098,12 +902,6 @@
       <c r="D33" t="n">
         <v>0.5267175572519084</v>
       </c>
-      <c r="E33" t="n">
-        <v>0.06451612903225806</v>
-      </c>
-      <c r="F33" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1118,12 +916,6 @@
       <c r="D34" t="n">
         <v>0.8931297709923665</v>
       </c>
-      <c r="E34" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1138,12 +930,6 @@
       <c r="D35" t="n">
         <v>0.6183206106870229</v>
       </c>
-      <c r="E35" t="n">
-        <v>0.08064516129032258</v>
-      </c>
-      <c r="F35" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1158,12 +944,6 @@
       <c r="D36" t="n">
         <v>0.4122137404580153</v>
       </c>
-      <c r="E36" t="n">
-        <v>0.2258064516129032</v>
-      </c>
-      <c r="F36" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1178,12 +958,6 @@
       <c r="D37" t="n">
         <v>0.6793893129770993</v>
       </c>
-      <c r="E37" t="n">
-        <v>0.2258064516129032</v>
-      </c>
-      <c r="F37" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1198,12 +972,6 @@
       <c r="D38" t="n">
         <v>0.7557251908396947</v>
       </c>
-      <c r="E38" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1218,12 +986,6 @@
       <c r="D39" t="n">
         <v>0.7175572519083969</v>
       </c>
-      <c r="E39" t="n">
-        <v>0.2580645161290323</v>
-      </c>
-      <c r="F39" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -1238,12 +1000,6 @@
       <c r="D40" t="n">
         <v>0.5877862595419847</v>
       </c>
-      <c r="E40" t="n">
-        <v>0.1290322580645161</v>
-      </c>
-      <c r="F40" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -1258,12 +1014,6 @@
       <c r="D41" t="n">
         <v>0.6106870229007634</v>
       </c>
-      <c r="E41" t="n">
-        <v>0.1290322580645161</v>
-      </c>
-      <c r="F41" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -1278,12 +1028,6 @@
       <c r="D42" t="n">
         <v>0.5419847328244275</v>
       </c>
-      <c r="E42" t="n">
-        <v>0.2419354838709677</v>
-      </c>
-      <c r="F42" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -1298,12 +1042,6 @@
       <c r="D43" t="n">
         <v>0.8320610687022901</v>
       </c>
-      <c r="E43" t="n">
-        <v>0.03225806451612903</v>
-      </c>
-      <c r="F43" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1318,12 +1056,6 @@
       <c r="D44" t="n">
         <v>0.5877862595419847</v>
       </c>
-      <c r="E44" t="n">
-        <v>0.4838709677419354</v>
-      </c>
-      <c r="F44" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1338,12 +1070,6 @@
       <c r="D45" t="n">
         <v>0.5496183206106871</v>
       </c>
-      <c r="E45" t="n">
-        <v>0.06451612903225806</v>
-      </c>
-      <c r="F45" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1358,12 +1084,6 @@
       <c r="D46" t="n">
         <v>0.8473282442748091</v>
       </c>
-      <c r="E46" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -1378,12 +1098,6 @@
       <c r="D47" t="n">
         <v>0.7709923664122137</v>
       </c>
-      <c r="E47" t="n">
-        <v>0.03225806451612903</v>
-      </c>
-      <c r="F47" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -1398,12 +1112,6 @@
       <c r="D48" t="n">
         <v>0.8320610687022901</v>
       </c>
-      <c r="E48" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -1418,12 +1126,6 @@
       <c r="D49" t="n">
         <v>0.648854961832061</v>
       </c>
-      <c r="E49" t="n">
-        <v>0</v>
-      </c>
-      <c r="F49" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -1438,12 +1140,6 @@
       <c r="D50" t="n">
         <v>0.3358778625954199</v>
       </c>
-      <c r="E50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F50" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1458,12 +1154,6 @@
       <c r="D51" t="n">
         <v>0.6793893129770993</v>
       </c>
-      <c r="E51" t="n">
-        <v>0</v>
-      </c>
-      <c r="F51" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -1478,12 +1168,6 @@
       <c r="D52" t="n">
         <v>0.5954198473282443</v>
       </c>
-      <c r="E52" t="n">
-        <v>0.08064516129032258</v>
-      </c>
-      <c r="F52" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -1498,12 +1182,6 @@
       <c r="D53" t="n">
         <v>0.6106870229007634</v>
       </c>
-      <c r="E53" t="n">
-        <v>0.06451612903225806</v>
-      </c>
-      <c r="F53" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -1518,12 +1196,6 @@
       <c r="D54" t="n">
         <v>0.5725190839694656</v>
       </c>
-      <c r="E54" t="n">
-        <v>0.2903225806451613</v>
-      </c>
-      <c r="F54" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1538,12 +1210,6 @@
       <c r="D55" t="n">
         <v>0.7938931297709924</v>
       </c>
-      <c r="E55" t="n">
-        <v>0.09677419354838709</v>
-      </c>
-      <c r="F55" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -1558,12 +1224,6 @@
       <c r="D56" t="n">
         <v>0.7709923664122137</v>
       </c>
-      <c r="E56" t="n">
-        <v>0</v>
-      </c>
-      <c r="F56" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -1578,12 +1238,6 @@
       <c r="D57" t="n">
         <v>0.6641221374045801</v>
       </c>
-      <c r="E57" t="n">
-        <v>0.1290322580645161</v>
-      </c>
-      <c r="F57" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -1598,12 +1252,6 @@
       <c r="D58" t="n">
         <v>0.8778625954198473</v>
       </c>
-      <c r="E58" t="n">
-        <v>0</v>
-      </c>
-      <c r="F58" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -1618,12 +1266,6 @@
       <c r="D59" t="n">
         <v>0.8702290076335878</v>
       </c>
-      <c r="E59" t="n">
-        <v>0</v>
-      </c>
-      <c r="F59" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -1638,12 +1280,6 @@
       <c r="D60" t="n">
         <v>0.7862595419847328</v>
       </c>
-      <c r="E60" t="n">
-        <v>0</v>
-      </c>
-      <c r="F60" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -1658,12 +1294,6 @@
       <c r="D61" t="n">
         <v>0.6717557251908397</v>
       </c>
-      <c r="E61" t="n">
-        <v>0</v>
-      </c>
-      <c r="F61" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -1678,12 +1308,6 @@
       <c r="D62" t="n">
         <v>0.4503816793893129</v>
       </c>
-      <c r="E62" t="n">
-        <v>0</v>
-      </c>
-      <c r="F62" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -1698,12 +1322,6 @@
       <c r="D63" t="n">
         <v>0.648854961832061</v>
       </c>
-      <c r="E63" t="n">
-        <v>0</v>
-      </c>
-      <c r="F63" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -1718,12 +1336,6 @@
       <c r="D64" t="n">
         <v>0.9083969465648855</v>
       </c>
-      <c r="E64" t="n">
-        <v>0</v>
-      </c>
-      <c r="F64" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -1738,12 +1350,6 @@
       <c r="D65" t="n">
         <v>0.4656488549618321</v>
       </c>
-      <c r="E65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F65" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -1758,12 +1364,6 @@
       <c r="D66" t="n">
         <v>0.7175572519083969</v>
       </c>
-      <c r="E66" t="n">
-        <v>0</v>
-      </c>
-      <c r="F66" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -1778,12 +1378,6 @@
       <c r="D67" t="n">
         <v>0.8473282442748091</v>
       </c>
-      <c r="E67" t="n">
-        <v>0.2258064516129032</v>
-      </c>
-      <c r="F67" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -1798,12 +1392,6 @@
       <c r="D68" t="n">
         <v>0.5496183206106871</v>
       </c>
-      <c r="E68" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F68" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -1818,12 +1406,6 @@
       <c r="D69" t="n">
         <v>0.7938931297709924</v>
       </c>
-      <c r="E69" t="n">
-        <v>0.09677419354838709</v>
-      </c>
-      <c r="F69" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -1838,12 +1420,6 @@
       <c r="D70" t="n">
         <v>0.7557251908396947</v>
       </c>
-      <c r="E70" t="n">
-        <v>0</v>
-      </c>
-      <c r="F70" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -1858,12 +1434,6 @@
       <c r="D71" t="n">
         <v>0.7022900763358778</v>
       </c>
-      <c r="E71" t="n">
-        <v>0</v>
-      </c>
-      <c r="F71" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -1878,12 +1448,6 @@
       <c r="D72" t="n">
         <v>0.5801526717557252</v>
       </c>
-      <c r="E72" t="n">
-        <v>0.06451612903225806</v>
-      </c>
-      <c r="F72" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -1898,12 +1462,6 @@
       <c r="D73" t="n">
         <v>0.6335877862595419</v>
       </c>
-      <c r="E73" t="n">
-        <v>0</v>
-      </c>
-      <c r="F73" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -1918,12 +1476,6 @@
       <c r="D74" t="n">
         <v>1</v>
       </c>
-      <c r="E74" t="n">
-        <v>0</v>
-      </c>
-      <c r="F74" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -1938,12 +1490,6 @@
       <c r="D75" t="n">
         <v>0.8778625954198473</v>
       </c>
-      <c r="E75" t="n">
-        <v>0</v>
-      </c>
-      <c r="F75" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -1958,12 +1504,6 @@
       <c r="D76" t="n">
         <v>0.7175572519083969</v>
       </c>
-      <c r="E76" t="n">
-        <v>0.03225806451612903</v>
-      </c>
-      <c r="F76" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -1978,12 +1518,6 @@
       <c r="D77" t="n">
         <v>0.6870229007633588</v>
       </c>
-      <c r="E77" t="n">
-        <v>0.2258064516129032</v>
-      </c>
-      <c r="F77" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -1998,12 +1532,6 @@
       <c r="D78" t="n">
         <v>0.7251908396946565</v>
       </c>
-      <c r="E78" t="n">
-        <v>0.3870967741935484</v>
-      </c>
-      <c r="F78" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -2018,12 +1546,6 @@
       <c r="D79" t="n">
         <v>0.7099236641221374</v>
       </c>
-      <c r="E79" t="n">
-        <v>0</v>
-      </c>
-      <c r="F79" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -2038,12 +1560,6 @@
       <c r="D80" t="n">
         <v>0.8625954198473282</v>
       </c>
-      <c r="E80" t="n">
-        <v>0</v>
-      </c>
-      <c r="F80" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -2058,12 +1574,6 @@
       <c r="D81" t="n">
         <v>0.6335877862595419</v>
       </c>
-      <c r="E81" t="n">
-        <v>0.09677419354838709</v>
-      </c>
-      <c r="F81" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -2078,12 +1588,6 @@
       <c r="D82" t="n">
         <v>0.8244274809160306</v>
       </c>
-      <c r="E82" t="n">
-        <v>0</v>
-      </c>
-      <c r="F82" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -2098,12 +1602,6 @@
       <c r="D83" t="n">
         <v>0.7557251908396947</v>
       </c>
-      <c r="E83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F83" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -2118,12 +1616,6 @@
       <c r="D84" t="n">
         <v>0.6793893129770993</v>
       </c>
-      <c r="E84" t="n">
-        <v>0</v>
-      </c>
-      <c r="F84" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -2138,12 +1630,6 @@
       <c r="D85" t="n">
         <v>0.816793893129771</v>
       </c>
-      <c r="E85" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F85" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -2158,12 +1644,6 @@
       <c r="D86" t="n">
         <v>0.3893129770992366</v>
       </c>
-      <c r="E86" t="n">
-        <v>0.09677419354838709</v>
-      </c>
-      <c r="F86" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -2178,12 +1658,6 @@
       <c r="D87" t="n">
         <v>0.6793893129770993</v>
       </c>
-      <c r="E87" t="n">
-        <v>0.2580645161290323</v>
-      </c>
-      <c r="F87" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -2198,12 +1672,6 @@
       <c r="D88" t="n">
         <v>0.6106870229007634</v>
       </c>
-      <c r="E88" t="n">
-        <v>0.1612903225806452</v>
-      </c>
-      <c r="F88" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -2218,12 +1686,6 @@
       <c r="D89" t="n">
         <v>0.648854961832061</v>
       </c>
-      <c r="E89" t="n">
-        <v>0</v>
-      </c>
-      <c r="F89" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -2238,12 +1700,6 @@
       <c r="D90" t="n">
         <v>0.6641221374045801</v>
       </c>
-      <c r="E90" t="n">
-        <v>0.2580645161290323</v>
-      </c>
-      <c r="F90" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -2258,12 +1714,6 @@
       <c r="D91" t="n">
         <v>0.3893129770992366</v>
       </c>
-      <c r="E91" t="n">
-        <v>0.1612903225806452</v>
-      </c>
-      <c r="F91" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -2278,12 +1728,6 @@
       <c r="D92" t="n">
         <v>0.7938931297709924</v>
       </c>
-      <c r="E92" t="n">
-        <v>0</v>
-      </c>
-      <c r="F92" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -2298,12 +1742,6 @@
       <c r="D93" t="n">
         <v>0.7404580152671756</v>
       </c>
-      <c r="E93" t="n">
-        <v>0</v>
-      </c>
-      <c r="F93" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -2318,12 +1756,6 @@
       <c r="D94" t="n">
         <v>0.7480916030534351</v>
       </c>
-      <c r="E94" t="n">
-        <v>0</v>
-      </c>
-      <c r="F94" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -2338,12 +1770,6 @@
       <c r="D95" t="n">
         <v>0.6717557251908397</v>
       </c>
-      <c r="E95" t="n">
-        <v>0</v>
-      </c>
-      <c r="F95" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -2358,12 +1784,6 @@
       <c r="D96" t="n">
         <v>0.5114503816793893</v>
       </c>
-      <c r="E96" t="n">
-        <v>0</v>
-      </c>
-      <c r="F96" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -2378,12 +1798,6 @@
       <c r="D97" t="n">
         <v>0.3053435114503817</v>
       </c>
-      <c r="E97" t="n">
-        <v>0</v>
-      </c>
-      <c r="F97" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -2398,12 +1812,6 @@
       <c r="D98" t="n">
         <v>0.6564885496183206</v>
       </c>
-      <c r="E98" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F98" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -2418,12 +1826,6 @@
       <c r="D99" t="n">
         <v>0.5801526717557252</v>
       </c>
-      <c r="E99" t="n">
-        <v>0.01612903225806452</v>
-      </c>
-      <c r="F99" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -2438,12 +1840,6 @@
       <c r="D100" t="n">
         <v>0.6946564885496184</v>
       </c>
-      <c r="E100" t="n">
-        <v>0.3064516129032258</v>
-      </c>
-      <c r="F100" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -2458,12 +1854,6 @@
       <c r="D101" t="n">
         <v>0.7786259541984732</v>
       </c>
-      <c r="E101" t="n">
-        <v>0</v>
-      </c>
-      <c r="F101" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -2478,12 +1868,6 @@
       <c r="D102" t="n">
         <v>0.816793893129771</v>
       </c>
-      <c r="E102" t="n">
-        <v>0.1290322580645161</v>
-      </c>
-      <c r="F102" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -2498,12 +1882,6 @@
       <c r="D103" t="n">
         <v>0.5648854961832062</v>
       </c>
-      <c r="E103" t="n">
-        <v>0.6774193548387097</v>
-      </c>
-      <c r="F103" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -2518,12 +1896,6 @@
       <c r="D104" t="n">
         <v>0.8244274809160306</v>
       </c>
-      <c r="E104" t="n">
-        <v>0</v>
-      </c>
-      <c r="F104" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -2538,12 +1910,6 @@
       <c r="D105" t="n">
         <v>0.9389312977099237</v>
       </c>
-      <c r="E105" t="n">
-        <v>0.1290322580645161</v>
-      </c>
-      <c r="F105" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -2558,12 +1924,6 @@
       <c r="D106" t="n">
         <v>0.7022900763358778</v>
       </c>
-      <c r="E106" t="n">
-        <v>0</v>
-      </c>
-      <c r="F106" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -2578,12 +1938,6 @@
       <c r="D107" t="n">
         <v>0.3358778625954199</v>
       </c>
-      <c r="E107" t="n">
-        <v>0.2419354838709677</v>
-      </c>
-      <c r="F107" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -2598,12 +1952,6 @@
       <c r="D108" t="n">
         <v>0.4580152671755725</v>
       </c>
-      <c r="E108" t="n">
-        <v>0.01612903225806452</v>
-      </c>
-      <c r="F108" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -2618,12 +1966,6 @@
       <c r="D109" t="n">
         <v>0.6183206106870229</v>
       </c>
-      <c r="E109" t="n">
-        <v>0.03225806451612903</v>
-      </c>
-      <c r="F109" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -2638,12 +1980,6 @@
       <c r="D110" t="n">
         <v>0.6946564885496184</v>
       </c>
-      <c r="E110" t="n">
-        <v>0.1774193548387097</v>
-      </c>
-      <c r="F110" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -2658,12 +1994,6 @@
       <c r="D111" t="n">
         <v>0.6717557251908397</v>
       </c>
-      <c r="E111" t="n">
-        <v>0</v>
-      </c>
-      <c r="F111" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -2678,12 +2008,6 @@
       <c r="D112" t="n">
         <v>0.6335877862595419</v>
       </c>
-      <c r="E112" t="n">
-        <v>0</v>
-      </c>
-      <c r="F112" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -2698,12 +2022,6 @@
       <c r="D113" t="n">
         <v>0.7786259541984732</v>
       </c>
-      <c r="E113" t="n">
-        <v>0.03225806451612903</v>
-      </c>
-      <c r="F113" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -2718,12 +2036,6 @@
       <c r="D114" t="n">
         <v>0.4732824427480916</v>
       </c>
-      <c r="E114" t="n">
-        <v>0.03225806451612903</v>
-      </c>
-      <c r="F114" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -2738,12 +2050,6 @@
       <c r="D115" t="n">
         <v>0.6870229007633588</v>
       </c>
-      <c r="E115" t="n">
-        <v>0</v>
-      </c>
-      <c r="F115" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -2758,12 +2064,6 @@
       <c r="D116" t="n">
         <v>0.6412213740458015</v>
       </c>
-      <c r="E116" t="n">
-        <v>0</v>
-      </c>
-      <c r="F116" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -2778,12 +2078,6 @@
       <c r="D117" t="n">
         <v>0.7557251908396947</v>
       </c>
-      <c r="E117" t="n">
-        <v>0</v>
-      </c>
-      <c r="F117" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -2798,12 +2092,6 @@
       <c r="D118" t="n">
         <v>0.7404580152671756</v>
       </c>
-      <c r="E118" t="n">
-        <v>0.3225806451612903</v>
-      </c>
-      <c r="F118" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -2818,12 +2106,6 @@
       <c r="D119" t="n">
         <v>0.6946564885496184</v>
       </c>
-      <c r="E119" t="n">
-        <v>0.3064516129032258</v>
-      </c>
-      <c r="F119" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -2838,12 +2120,6 @@
       <c r="D120" t="n">
         <v>0.7709923664122137</v>
       </c>
-      <c r="E120" t="n">
-        <v>0</v>
-      </c>
-      <c r="F120" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -2858,12 +2134,6 @@
       <c r="D121" t="n">
         <v>0.6183206106870229</v>
       </c>
-      <c r="E121" t="n">
-        <v>0</v>
-      </c>
-      <c r="F121" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -2878,12 +2148,6 @@
       <c r="D122" t="n">
         <v>0.3893129770992366</v>
       </c>
-      <c r="E122" t="n">
-        <v>0.3225806451612903</v>
-      </c>
-      <c r="F122" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -2898,12 +2162,6 @@
       <c r="D123" t="n">
         <v>0.8473282442748091</v>
       </c>
-      <c r="E123" t="n">
-        <v>0</v>
-      </c>
-      <c r="F123" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -2918,12 +2176,6 @@
       <c r="D124" t="n">
         <v>0.7709923664122137</v>
       </c>
-      <c r="E124" t="n">
-        <v>0</v>
-      </c>
-      <c r="F124" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -2938,12 +2190,6 @@
       <c r="D125" t="n">
         <v>0.732824427480916</v>
       </c>
-      <c r="E125" t="n">
-        <v>0</v>
-      </c>
-      <c r="F125" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -2958,12 +2204,6 @@
       <c r="D126" t="n">
         <v>0.8244274809160306</v>
       </c>
-      <c r="E126" t="n">
-        <v>0</v>
-      </c>
-      <c r="F126" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -2978,12 +2218,6 @@
       <c r="D127" t="n">
         <v>0.9236641221374046</v>
       </c>
-      <c r="E127" t="n">
-        <v>0.1129032258064516</v>
-      </c>
-      <c r="F127" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -2998,12 +2232,6 @@
       <c r="D128" t="n">
         <v>0.5496183206106871</v>
       </c>
-      <c r="E128" t="n">
-        <v>0.01612903225806452</v>
-      </c>
-      <c r="F128" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -3018,12 +2246,6 @@
       <c r="D129" t="n">
         <v>0.7709923664122137</v>
       </c>
-      <c r="E129" t="n">
-        <v>0</v>
-      </c>
-      <c r="F129" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -3038,12 +2260,6 @@
       <c r="D130" t="n">
         <v>0.7480916030534351</v>
       </c>
-      <c r="E130" t="n">
-        <v>0.01612903225806452</v>
-      </c>
-      <c r="F130" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -3058,12 +2274,6 @@
       <c r="D131" t="n">
         <v>0.3816793893129771</v>
       </c>
-      <c r="E131" t="n">
-        <v>0.03225806451612903</v>
-      </c>
-      <c r="F131" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -3078,12 +2288,6 @@
       <c r="D132" t="n">
         <v>0.7022900763358778</v>
       </c>
-      <c r="E132" t="n">
-        <v>0</v>
-      </c>
-      <c r="F132" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -3098,12 +2302,6 @@
       <c r="D133" t="n">
         <v>0.6946564885496184</v>
       </c>
-      <c r="E133" t="n">
-        <v>0</v>
-      </c>
-      <c r="F133" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -3118,12 +2316,6 @@
       <c r="D134" t="n">
         <v>0.6946564885496184</v>
       </c>
-      <c r="E134" t="n">
-        <v>0</v>
-      </c>
-      <c r="F134" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -3138,12 +2330,6 @@
       <c r="D135" t="n">
         <v>0.6259541984732825</v>
       </c>
-      <c r="E135" t="n">
-        <v>0</v>
-      </c>
-      <c r="F135" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -3158,12 +2344,6 @@
       <c r="D136" t="n">
         <v>0.7022900763358778</v>
       </c>
-      <c r="E136" t="n">
-        <v>0</v>
-      </c>
-      <c r="F136" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -3178,12 +2358,6 @@
       <c r="D137" t="n">
         <v>0.7022900763358778</v>
       </c>
-      <c r="E137" t="n">
-        <v>0</v>
-      </c>
-      <c r="F137" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -3198,12 +2372,6 @@
       <c r="D138" t="n">
         <v>0.1908396946564886</v>
       </c>
-      <c r="E138" t="n">
-        <v>0</v>
-      </c>
-      <c r="F138" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -3218,12 +2386,6 @@
       <c r="D139" t="n">
         <v>0.5267175572519084</v>
       </c>
-      <c r="E139" t="n">
-        <v>0</v>
-      </c>
-      <c r="F139" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -3238,12 +2400,6 @@
       <c r="D140" t="n">
         <v>0.4198473282442748</v>
       </c>
-      <c r="E140" t="n">
-        <v>0.2419354838709677</v>
-      </c>
-      <c r="F140" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -3258,12 +2414,6 @@
       <c r="D141" t="n">
         <v>0.2595419847328244</v>
       </c>
-      <c r="E141" t="n">
-        <v>0.03225806451612903</v>
-      </c>
-      <c r="F141" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -3278,12 +2428,6 @@
       <c r="D142" t="n">
         <v>0.6564885496183206</v>
       </c>
-      <c r="E142" t="n">
-        <v>0.09677419354838709</v>
-      </c>
-      <c r="F142" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -3298,12 +2442,6 @@
       <c r="D143" t="n">
         <v>0.8396946564885496</v>
       </c>
-      <c r="E143" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F143" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -3318,12 +2456,6 @@
       <c r="D144" t="n">
         <v>0.7786259541984732</v>
       </c>
-      <c r="E144" t="n">
-        <v>0</v>
-      </c>
-      <c r="F144" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -3338,12 +2470,6 @@
       <c r="D145" t="n">
         <v>0.5419847328244275</v>
       </c>
-      <c r="E145" t="n">
-        <v>0.04838709677419355</v>
-      </c>
-      <c r="F145" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -3358,12 +2484,6 @@
       <c r="D146" t="n">
         <v>0.3435114503816794</v>
       </c>
-      <c r="E146" t="n">
-        <v>0.1774193548387097</v>
-      </c>
-      <c r="F146" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -3378,12 +2498,6 @@
       <c r="D147" t="n">
         <v>0.5496183206106871</v>
       </c>
-      <c r="E147" t="n">
-        <v>0</v>
-      </c>
-      <c r="F147" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -3398,12 +2512,6 @@
       <c r="D148" t="n">
         <v>0.5954198473282443</v>
       </c>
-      <c r="E148" t="n">
-        <v>0.04838709677419355</v>
-      </c>
-      <c r="F148" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -3418,12 +2526,6 @@
       <c r="D149" t="n">
         <v>0.7633587786259542</v>
       </c>
-      <c r="E149" t="n">
-        <v>0.1451612903225807</v>
-      </c>
-      <c r="F149" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -3438,12 +2540,6 @@
       <c r="D150" t="n">
         <v>0.7480916030534351</v>
       </c>
-      <c r="E150" t="n">
-        <v>0</v>
-      </c>
-      <c r="F150" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -3458,12 +2554,6 @@
       <c r="D151" t="n">
         <v>0.6030534351145038</v>
       </c>
-      <c r="E151" t="n">
-        <v>0</v>
-      </c>
-      <c r="F151" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -3478,12 +2568,6 @@
       <c r="D152" t="n">
         <v>0.5114503816793893</v>
       </c>
-      <c r="E152" t="n">
-        <v>0.3709677419354838</v>
-      </c>
-      <c r="F152" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -3498,12 +2582,6 @@
       <c r="D153" t="n">
         <v>0.4122137404580153</v>
       </c>
-      <c r="E153" t="n">
-        <v>0.2580645161290323</v>
-      </c>
-      <c r="F153" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -3518,12 +2596,6 @@
       <c r="D154" t="n">
         <v>0.6412213740458015</v>
       </c>
-      <c r="E154" t="n">
-        <v>0.09677419354838709</v>
-      </c>
-      <c r="F154" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -3538,12 +2610,6 @@
       <c r="D155" t="n">
         <v>0.6183206106870229</v>
       </c>
-      <c r="E155" t="n">
-        <v>0</v>
-      </c>
-      <c r="F155" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -3558,12 +2624,6 @@
       <c r="D156" t="n">
         <v>0.6183206106870229</v>
       </c>
-      <c r="E156" t="n">
-        <v>0</v>
-      </c>
-      <c r="F156" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
@@ -3578,12 +2638,6 @@
       <c r="D157" t="n">
         <v>0.4580152671755725</v>
       </c>
-      <c r="E157" t="n">
-        <v>0.09677419354838709</v>
-      </c>
-      <c r="F157" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -3598,12 +2652,6 @@
       <c r="D158" t="n">
         <v>0.8244274809160306</v>
       </c>
-      <c r="E158" t="n">
-        <v>0</v>
-      </c>
-      <c r="F158" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -3618,12 +2666,6 @@
       <c r="D159" t="n">
         <v>0.7862595419847328</v>
       </c>
-      <c r="E159" t="n">
-        <v>0</v>
-      </c>
-      <c r="F159" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
@@ -3638,12 +2680,6 @@
       <c r="D160" t="n">
         <v>0.5572519083969466</v>
       </c>
-      <c r="E160" t="n">
-        <v>0.06451612903225806</v>
-      </c>
-      <c r="F160" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -3658,12 +2694,6 @@
       <c r="D161" t="n">
         <v>0.7022900763358778</v>
       </c>
-      <c r="E161" t="n">
-        <v>0</v>
-      </c>
-      <c r="F161" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -3678,12 +2708,6 @@
       <c r="D162" t="n">
         <v>0.7480916030534351</v>
       </c>
-      <c r="E162" t="n">
-        <v>0</v>
-      </c>
-      <c r="F162" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
@@ -3698,12 +2722,6 @@
       <c r="D163" t="n">
         <v>0.7251908396946565</v>
       </c>
-      <c r="E163" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F163" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -3718,12 +2736,6 @@
       <c r="D164" t="n">
         <v>0.8473282442748091</v>
       </c>
-      <c r="E164" t="n">
-        <v>0</v>
-      </c>
-      <c r="F164" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -3738,12 +2750,6 @@
       <c r="D165" t="n">
         <v>0.7786259541984732</v>
       </c>
-      <c r="E165" t="n">
-        <v>0</v>
-      </c>
-      <c r="F165" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -3758,12 +2764,6 @@
       <c r="D166" t="n">
         <v>0.7786259541984732</v>
       </c>
-      <c r="E166" t="n">
-        <v>0</v>
-      </c>
-      <c r="F166" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -3778,12 +2778,6 @@
       <c r="D167" t="n">
         <v>0.2824427480916031</v>
       </c>
-      <c r="E167" t="n">
-        <v>0.2419354838709677</v>
-      </c>
-      <c r="F167" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -3798,12 +2792,6 @@
       <c r="D168" t="n">
         <v>0.4427480916030535</v>
       </c>
-      <c r="E168" t="n">
-        <v>0.4193548387096774</v>
-      </c>
-      <c r="F168" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
@@ -3818,12 +2806,6 @@
       <c r="D169" t="n">
         <v>0.6793893129770993</v>
       </c>
-      <c r="E169" t="n">
-        <v>0.5806451612903226</v>
-      </c>
-      <c r="F169" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -3838,12 +2820,6 @@
       <c r="D170" t="n">
         <v>0.5801526717557252</v>
       </c>
-      <c r="E170" t="n">
-        <v>0.2258064516129032</v>
-      </c>
-      <c r="F170" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
@@ -3858,12 +2834,6 @@
       <c r="D171" t="n">
         <v>0.6412213740458015</v>
       </c>
-      <c r="E171" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F171" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
@@ -3878,12 +2848,6 @@
       <c r="D172" t="n">
         <v>0.5419847328244275</v>
       </c>
-      <c r="E172" t="n">
-        <v>0.09677419354838709</v>
-      </c>
-      <c r="F172" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
@@ -3898,12 +2862,6 @@
       <c r="D173" t="n">
         <v>0.7404580152671756</v>
       </c>
-      <c r="E173" t="n">
-        <v>0.1612903225806452</v>
-      </c>
-      <c r="F173" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
@@ -3918,12 +2876,6 @@
       <c r="D174" t="n">
         <v>0.6793893129770993</v>
       </c>
-      <c r="E174" t="n">
-        <v>0.2903225806451613</v>
-      </c>
-      <c r="F174" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
@@ -3938,12 +2890,6 @@
       <c r="D175" t="n">
         <v>0.7786259541984732</v>
       </c>
-      <c r="E175" t="n">
-        <v>0.5161290322580645</v>
-      </c>
-      <c r="F175" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
@@ -3958,12 +2904,6 @@
       <c r="D176" t="n">
         <v>0.4656488549618321</v>
       </c>
-      <c r="E176" t="n">
-        <v>0.3870967741935484</v>
-      </c>
-      <c r="F176" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
@@ -3978,12 +2918,6 @@
       <c r="D177" t="n">
         <v>0.3282442748091603</v>
       </c>
-      <c r="E177" t="n">
-        <v>0.3225806451612903</v>
-      </c>
-      <c r="F177" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
@@ -3998,12 +2932,6 @@
       <c r="D178" t="n">
         <v>0.6793893129770993</v>
       </c>
-      <c r="E178" t="n">
-        <v>0.2258064516129032</v>
-      </c>
-      <c r="F178" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
@@ -4018,12 +2946,6 @@
       <c r="D179" t="n">
         <v>0.6641221374045801</v>
       </c>
-      <c r="E179" t="n">
-        <v>0</v>
-      </c>
-      <c r="F179" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
@@ -4038,12 +2960,6 @@
       <c r="D180" t="n">
         <v>0.3740458015267176</v>
       </c>
-      <c r="E180" t="n">
-        <v>0.4032258064516129</v>
-      </c>
-      <c r="F180" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
@@ -4058,12 +2974,6 @@
       <c r="D181" t="n">
         <v>0.3129770992366412</v>
       </c>
-      <c r="E181" t="n">
-        <v>0.09677419354838709</v>
-      </c>
-      <c r="F181" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
@@ -4078,12 +2988,6 @@
       <c r="D182" t="n">
         <v>0.4656488549618321</v>
       </c>
-      <c r="E182" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F182" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
@@ -4098,12 +3002,6 @@
       <c r="D183" t="n">
         <v>0.3282442748091603</v>
       </c>
-      <c r="E183" t="n">
-        <v>0.1612903225806452</v>
-      </c>
-      <c r="F183" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
@@ -4118,12 +3016,6 @@
       <c r="D184" t="n">
         <v>0.7480916030534351</v>
       </c>
-      <c r="E184" t="n">
-        <v>0</v>
-      </c>
-      <c r="F184" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
@@ -4138,12 +3030,6 @@
       <c r="D185" t="n">
         <v>0.7175572519083969</v>
       </c>
-      <c r="E185" t="n">
-        <v>0.4032258064516129</v>
-      </c>
-      <c r="F185" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
@@ -4158,12 +3044,6 @@
       <c r="D186" t="n">
         <v>0.4351145038167939</v>
       </c>
-      <c r="E186" t="n">
-        <v>0.4193548387096774</v>
-      </c>
-      <c r="F186" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
@@ -4178,12 +3058,6 @@
       <c r="D187" t="n">
         <v>0.6259541984732825</v>
       </c>
-      <c r="E187" t="n">
-        <v>0</v>
-      </c>
-      <c r="F187" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
@@ -4198,12 +3072,6 @@
       <c r="D188" t="n">
         <v>0.5572519083969466</v>
       </c>
-      <c r="E188" t="n">
-        <v>0.2258064516129032</v>
-      </c>
-      <c r="F188" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
@@ -4218,12 +3086,6 @@
       <c r="D189" t="n">
         <v>0.2900763358778626</v>
       </c>
-      <c r="E189" t="n">
-        <v>0.3548387096774194</v>
-      </c>
-      <c r="F189" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
@@ -4238,12 +3100,6 @@
       <c r="D190" t="n">
         <v>0.7022900763358778</v>
       </c>
-      <c r="E190" t="n">
-        <v>0.09677419354838709</v>
-      </c>
-      <c r="F190" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
@@ -4258,12 +3114,6 @@
       <c r="D191" t="n">
         <v>0.6641221374045801</v>
       </c>
-      <c r="E191" t="n">
-        <v>0</v>
-      </c>
-      <c r="F191" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
@@ -4278,12 +3128,6 @@
       <c r="D192" t="n">
         <v>0.5419847328244275</v>
       </c>
-      <c r="E192" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F192" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
@@ -4298,12 +3142,6 @@
       <c r="D193" t="n">
         <v>0.4580152671755725</v>
       </c>
-      <c r="E193" t="n">
-        <v>0.3548387096774194</v>
-      </c>
-      <c r="F193" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
@@ -4318,12 +3156,6 @@
       <c r="D194" t="n">
         <v>0.3206106870229007</v>
       </c>
-      <c r="E194" t="n">
-        <v>0.2258064516129032</v>
-      </c>
-      <c r="F194" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
@@ -4338,12 +3170,6 @@
       <c r="D195" t="n">
         <v>0.5419847328244275</v>
       </c>
-      <c r="E195" t="n">
-        <v>0.4516129032258064</v>
-      </c>
-      <c r="F195" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
@@ -4358,12 +3184,6 @@
       <c r="D196" t="n">
         <v>0.6412213740458015</v>
       </c>
-      <c r="E196" t="n">
-        <v>0.4838709677419354</v>
-      </c>
-      <c r="F196" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
@@ -4378,12 +3198,6 @@
       <c r="D197" t="n">
         <v>0.5267175572519084</v>
       </c>
-      <c r="E197" t="n">
-        <v>0.5483870967741935</v>
-      </c>
-      <c r="F197" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
@@ -4398,12 +3212,6 @@
       <c r="D198" t="n">
         <v>0.5801526717557252</v>
       </c>
-      <c r="E198" t="n">
-        <v>0.5806451612903226</v>
-      </c>
-      <c r="F198" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
@@ -4418,12 +3226,6 @@
       <c r="D199" t="n">
         <v>0.7022900763358778</v>
       </c>
-      <c r="E199" t="n">
-        <v>0.03225806451612903</v>
-      </c>
-      <c r="F199" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
@@ -4438,12 +3240,6 @@
       <c r="D200" t="n">
         <v>0.2137404580152672</v>
       </c>
-      <c r="E200" t="n">
-        <v>0.2903225806451613</v>
-      </c>
-      <c r="F200" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
@@ -4458,12 +3254,6 @@
       <c r="D201" t="n">
         <v>0.6641221374045801</v>
       </c>
-      <c r="E201" t="n">
-        <v>0.09677419354838709</v>
-      </c>
-      <c r="F201" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
@@ -4478,12 +3268,6 @@
       <c r="D202" t="n">
         <v>0.8091603053435115</v>
       </c>
-      <c r="E202" t="n">
-        <v>0</v>
-      </c>
-      <c r="F202" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
@@ -4498,12 +3282,6 @@
       <c r="D203" t="n">
         <v>0.5343511450381679</v>
       </c>
-      <c r="E203" t="n">
-        <v>0.4516129032258064</v>
-      </c>
-      <c r="F203" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
@@ -4518,12 +3296,6 @@
       <c r="D204" t="n">
         <v>0.3053435114503817</v>
       </c>
-      <c r="E204" t="n">
-        <v>0.1290322580645161</v>
-      </c>
-      <c r="F204" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
@@ -4538,12 +3310,6 @@
       <c r="D205" t="n">
         <v>0.6030534351145038</v>
       </c>
-      <c r="E205" t="n">
-        <v>0.2580645161290323</v>
-      </c>
-      <c r="F205" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
@@ -4558,12 +3324,6 @@
       <c r="D206" t="n">
         <v>0.5648854961832062</v>
       </c>
-      <c r="E206" t="n">
-        <v>1</v>
-      </c>
-      <c r="F206" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
@@ -4578,12 +3338,6 @@
       <c r="D207" t="n">
         <v>0.6870229007633588</v>
       </c>
-      <c r="E207" t="n">
-        <v>0</v>
-      </c>
-      <c r="F207" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
@@ -4598,12 +3352,6 @@
       <c r="D208" t="n">
         <v>0.5419847328244275</v>
       </c>
-      <c r="E208" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F208" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
@@ -4618,12 +3366,6 @@
       <c r="D209" t="n">
         <v>0.6564885496183206</v>
       </c>
-      <c r="E209" t="n">
-        <v>0.4193548387096774</v>
-      </c>
-      <c r="F209" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
@@ -4638,12 +3380,6 @@
       <c r="D210" t="n">
         <v>0.5190839694656488</v>
       </c>
-      <c r="E210" t="n">
-        <v>0.3225806451612903</v>
-      </c>
-      <c r="F210" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
@@ -4658,12 +3394,6 @@
       <c r="D211" t="n">
         <v>0.6946564885496184</v>
       </c>
-      <c r="E211" t="n">
-        <v>0</v>
-      </c>
-      <c r="F211" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
@@ -4678,12 +3408,6 @@
       <c r="D212" t="n">
         <v>0.6030534351145038</v>
       </c>
-      <c r="E212" t="n">
-        <v>0.06451612903225806</v>
-      </c>
-      <c r="F212" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
@@ -4698,12 +3422,6 @@
       <c r="D213" t="n">
         <v>0.5267175572519084</v>
       </c>
-      <c r="E213" t="n">
-        <v>0.5806451612903226</v>
-      </c>
-      <c r="F213" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
@@ -4718,12 +3436,6 @@
       <c r="D214" t="n">
         <v>0.5267175572519084</v>
       </c>
-      <c r="E214" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F214" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
@@ -4738,12 +3450,6 @@
       <c r="D215" t="n">
         <v>0.5725190839694656</v>
       </c>
-      <c r="E215" t="n">
-        <v>0.1612903225806452</v>
-      </c>
-      <c r="F215" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
@@ -4758,12 +3464,6 @@
       <c r="D216" t="n">
         <v>0.5572519083969466</v>
       </c>
-      <c r="E216" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F216" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="217">
       <c r="A217" t="n">
@@ -4778,12 +3478,6 @@
       <c r="D217" t="n">
         <v>0.4961832061068702</v>
       </c>
-      <c r="E217" t="n">
-        <v>0.4838709677419354</v>
-      </c>
-      <c r="F217" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="218">
       <c r="A218" t="n">
@@ -4798,12 +3492,6 @@
       <c r="D218" t="n">
         <v>0.1984732824427481</v>
       </c>
-      <c r="E218" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F218" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
@@ -4818,12 +3506,6 @@
       <c r="D219" t="n">
         <v>0.4656488549618321</v>
       </c>
-      <c r="E219" t="n">
-        <v>0.2903225806451613</v>
-      </c>
-      <c r="F219" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
@@ -4838,12 +3520,6 @@
       <c r="D220" t="n">
         <v>0.4274809160305343</v>
       </c>
-      <c r="E220" t="n">
-        <v>0.4516129032258064</v>
-      </c>
-      <c r="F220" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="221">
       <c r="A221" t="n">
@@ -4858,12 +3534,6 @@
       <c r="D221" t="n">
         <v>0.6030534351145038</v>
       </c>
-      <c r="E221" t="n">
-        <v>0</v>
-      </c>
-      <c r="F221" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
@@ -4878,12 +3548,6 @@
       <c r="D222" t="n">
         <v>0.6335877862595419</v>
       </c>
-      <c r="E222" t="n">
-        <v>0.6451612903225806</v>
-      </c>
-      <c r="F222" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
@@ -4898,12 +3562,6 @@
       <c r="D223" t="n">
         <v>0.3053435114503817</v>
       </c>
-      <c r="E223" t="n">
-        <v>0.9032258064516128</v>
-      </c>
-      <c r="F223" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="224">
       <c r="A224" t="n">
@@ -4918,12 +3576,6 @@
       <c r="D224" t="n">
         <v>0.7862595419847328</v>
       </c>
-      <c r="E224" t="n">
-        <v>0.2258064516129032</v>
-      </c>
-      <c r="F224" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="225">
       <c r="A225" t="n">
@@ -4938,12 +3590,6 @@
       <c r="D225" t="n">
         <v>0.4732824427480916</v>
       </c>
-      <c r="E225" t="n">
-        <v>0.6451612903225806</v>
-      </c>
-      <c r="F225" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
@@ -4958,12 +3604,6 @@
       <c r="D226" t="n">
         <v>0.4198473282442748</v>
       </c>
-      <c r="E226" t="n">
-        <v>0.4516129032258064</v>
-      </c>
-      <c r="F226" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
@@ -4978,12 +3618,6 @@
       <c r="D227" t="n">
         <v>0.4122137404580153</v>
       </c>
-      <c r="E227" t="n">
-        <v>0.4193548387096774</v>
-      </c>
-      <c r="F227" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="228">
       <c r="A228" t="n">
@@ -4998,12 +3632,6 @@
       <c r="D228" t="n">
         <v>0.2442748091603053</v>
       </c>
-      <c r="E228" t="n">
-        <v>0.2258064516129032</v>
-      </c>
-      <c r="F228" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
@@ -5018,12 +3646,6 @@
       <c r="D229" t="n">
         <v>0.4503816793893129</v>
       </c>
-      <c r="E229" t="n">
-        <v>0.2580645161290323</v>
-      </c>
-      <c r="F229" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="230">
       <c r="A230" t="n">
@@ -5038,12 +3660,6 @@
       <c r="D230" t="n">
         <v>0.6717557251908397</v>
       </c>
-      <c r="E230" t="n">
-        <v>0.03225806451612903</v>
-      </c>
-      <c r="F230" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="231">
       <c r="A231" t="n">
@@ -5058,12 +3674,6 @@
       <c r="D231" t="n">
         <v>0.4580152671755725</v>
       </c>
-      <c r="E231" t="n">
-        <v>0.2903225806451613</v>
-      </c>
-      <c r="F231" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="232">
       <c r="A232" t="n">
@@ -5078,12 +3688,6 @@
       <c r="D232" t="n">
         <v>0.6183206106870229</v>
       </c>
-      <c r="E232" t="n">
-        <v>0</v>
-      </c>
-      <c r="F232" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="233">
       <c r="A233" t="n">
@@ -5098,12 +3702,6 @@
       <c r="D233" t="n">
         <v>0.4045801526717557</v>
       </c>
-      <c r="E233" t="n">
-        <v>0.1612903225806452</v>
-      </c>
-      <c r="F233" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
@@ -5118,12 +3716,6 @@
       <c r="D234" t="n">
         <v>0.5648854961832062</v>
       </c>
-      <c r="E234" t="n">
-        <v>0.1290322580645161</v>
-      </c>
-      <c r="F234" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
@@ -5138,12 +3730,6 @@
       <c r="D235" t="n">
         <v>0.1908396946564886</v>
       </c>
-      <c r="E235" t="n">
-        <v>0.3548387096774194</v>
-      </c>
-      <c r="F235" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="236">
       <c r="A236" t="n">
@@ -5158,12 +3744,6 @@
       <c r="D236" t="n">
         <v>0.2900763358778626</v>
       </c>
-      <c r="E236" t="n">
-        <v>0.3870967741935484</v>
-      </c>
-      <c r="F236" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
@@ -5178,12 +3758,6 @@
       <c r="D237" t="n">
         <v>0.7786259541984732</v>
       </c>
-      <c r="E237" t="n">
-        <v>0.2580645161290323</v>
-      </c>
-      <c r="F237" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
@@ -5198,12 +3772,6 @@
       <c r="D238" t="n">
         <v>0.7633587786259542</v>
       </c>
-      <c r="E238" t="n">
-        <v>0</v>
-      </c>
-      <c r="F238" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
@@ -5218,12 +3786,6 @@
       <c r="D239" t="n">
         <v>0.7557251908396947</v>
       </c>
-      <c r="E239" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F239" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
@@ -5238,12 +3800,6 @@
       <c r="D240" t="n">
         <v>0.6946564885496184</v>
       </c>
-      <c r="E240" t="n">
-        <v>0</v>
-      </c>
-      <c r="F240" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
@@ -5258,12 +3814,6 @@
       <c r="D241" t="n">
         <v>0.648854961832061</v>
       </c>
-      <c r="E241" t="n">
-        <v>0</v>
-      </c>
-      <c r="F241" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
@@ -5278,12 +3828,6 @@
       <c r="D242" t="n">
         <v>0.3129770992366412</v>
       </c>
-      <c r="E242" t="n">
-        <v>0.4677419354838709</v>
-      </c>
-      <c r="F242" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
@@ -5298,12 +3842,6 @@
       <c r="D243" t="n">
         <v>0.5496183206106871</v>
       </c>
-      <c r="E243" t="n">
-        <v>0</v>
-      </c>
-      <c r="F243" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
@@ -5318,12 +3856,6 @@
       <c r="D244" t="n">
         <v>0.4656488549618321</v>
       </c>
-      <c r="E244" t="n">
-        <v>0.3225806451612903</v>
-      </c>
-      <c r="F244" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
@@ -5338,12 +3870,6 @@
       <c r="D245" t="n">
         <v>0.1297709923664122</v>
       </c>
-      <c r="E245" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F245" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
@@ -5358,12 +3884,6 @@
       <c r="D246" t="n">
         <v>0.2595419847328244</v>
       </c>
-      <c r="E246" t="n">
-        <v>0.3387096774193549</v>
-      </c>
-      <c r="F246" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="247">
       <c r="A247" t="n">
@@ -5378,12 +3898,6 @@
       <c r="D247" t="n">
         <v>0.7251908396946565</v>
       </c>
-      <c r="E247" t="n">
-        <v>0.08064516129032258</v>
-      </c>
-      <c r="F247" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
@@ -5398,12 +3912,6 @@
       <c r="D248" t="n">
         <v>0.6030534351145038</v>
       </c>
-      <c r="E248" t="n">
-        <v>0.3064516129032258</v>
-      </c>
-      <c r="F248" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
@@ -5418,12 +3926,6 @@
       <c r="D249" t="n">
         <v>0.3740458015267176</v>
       </c>
-      <c r="E249" t="n">
-        <v>0</v>
-      </c>
-      <c r="F249" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
@@ -5438,12 +3940,6 @@
       <c r="D250" t="n">
         <v>0.9465648854961832</v>
       </c>
-      <c r="E250" t="n">
-        <v>0</v>
-      </c>
-      <c r="F250" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
@@ -5458,12 +3954,6 @@
       <c r="D251" t="n">
         <v>0.5725190839694656</v>
       </c>
-      <c r="E251" t="n">
-        <v>0.3225806451612903</v>
-      </c>
-      <c r="F251" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
@@ -5478,12 +3968,6 @@
       <c r="D252" t="n">
         <v>0.3893129770992366</v>
       </c>
-      <c r="E252" t="n">
-        <v>0.6774193548387097</v>
-      </c>
-      <c r="F252" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
@@ -5498,12 +3982,6 @@
       <c r="D253" t="n">
         <v>0.5496183206106871</v>
       </c>
-      <c r="E253" t="n">
-        <v>0.01612903225806452</v>
-      </c>
-      <c r="F253" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
@@ -5518,12 +3996,6 @@
       <c r="D254" t="n">
         <v>0.267175572519084</v>
       </c>
-      <c r="E254" t="n">
-        <v>0.3064516129032258</v>
-      </c>
-      <c r="F254" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
@@ -5538,12 +4010,6 @@
       <c r="D255" t="n">
         <v>0.4122137404580153</v>
       </c>
-      <c r="E255" t="n">
-        <v>0.1451612903225807</v>
-      </c>
-      <c r="F255" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
@@ -5558,12 +4024,6 @@
       <c r="D256" t="n">
         <v>0.4122137404580153</v>
       </c>
-      <c r="E256" t="n">
-        <v>0</v>
-      </c>
-      <c r="F256" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
@@ -5578,12 +4038,6 @@
       <c r="D257" t="n">
         <v>0.5801526717557252</v>
       </c>
-      <c r="E257" t="n">
-        <v>0</v>
-      </c>
-      <c r="F257" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
@@ -5598,12 +4052,6 @@
       <c r="D258" t="n">
         <v>0.4503816793893129</v>
       </c>
-      <c r="E258" t="n">
-        <v>0.4838709677419354</v>
-      </c>
-      <c r="F258" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
@@ -5618,12 +4066,6 @@
       <c r="D259" t="n">
         <v>0.4198473282442748</v>
       </c>
-      <c r="E259" t="n">
-        <v>0.1451612903225807</v>
-      </c>
-      <c r="F259" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
@@ -5638,12 +4080,6 @@
       <c r="D260" t="n">
         <v>0.6335877862595419</v>
       </c>
-      <c r="E260" t="n">
-        <v>0.2258064516129032</v>
-      </c>
-      <c r="F260" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
@@ -5658,12 +4094,6 @@
       <c r="D261" t="n">
         <v>0.8473282442748091</v>
       </c>
-      <c r="E261" t="n">
-        <v>0.6129032258064515</v>
-      </c>
-      <c r="F261" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
@@ -5678,12 +4108,6 @@
       <c r="D262" t="n">
         <v>0.7175572519083969</v>
       </c>
-      <c r="E262" t="n">
-        <v>0.1612903225806452</v>
-      </c>
-      <c r="F262" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
@@ -5698,12 +4122,6 @@
       <c r="D263" t="n">
         <v>0.6793893129770993</v>
       </c>
-      <c r="E263" t="n">
-        <v>0</v>
-      </c>
-      <c r="F263" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
@@ -5718,12 +4136,6 @@
       <c r="D264" t="n">
         <v>0.183206106870229</v>
       </c>
-      <c r="E264" t="n">
-        <v>0.3225806451612903</v>
-      </c>
-      <c r="F264" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
@@ -5738,12 +4150,6 @@
       <c r="D265" t="n">
         <v>0.7480916030534351</v>
       </c>
-      <c r="E265" t="n">
-        <v>0.2903225806451613</v>
-      </c>
-      <c r="F265" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
@@ -5758,12 +4164,6 @@
       <c r="D266" t="n">
         <v>0.2824427480916031</v>
       </c>
-      <c r="E266" t="n">
-        <v>0</v>
-      </c>
-      <c r="F266" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
@@ -5778,12 +4178,6 @@
       <c r="D267" t="n">
         <v>0.4656488549618321</v>
       </c>
-      <c r="E267" t="n">
-        <v>0.01612903225806452</v>
-      </c>
-      <c r="F267" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
@@ -5798,12 +4192,6 @@
       <c r="D268" t="n">
         <v>0.3511450381679389</v>
       </c>
-      <c r="E268" t="n">
-        <v>0.5483870967741935</v>
-      </c>
-      <c r="F268" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
@@ -5818,12 +4206,6 @@
       <c r="D269" t="n">
         <v>0.4198473282442748</v>
       </c>
-      <c r="E269" t="n">
-        <v>0.1290322580645161</v>
-      </c>
-      <c r="F269" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="270">
       <c r="A270" t="n">
@@ -5838,12 +4220,6 @@
       <c r="D270" t="n">
         <v>0.3435114503816794</v>
       </c>
-      <c r="E270" t="n">
-        <v>0.5161290322580645</v>
-      </c>
-      <c r="F270" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="271">
       <c r="A271" t="n">
@@ -5858,12 +4234,6 @@
       <c r="D271" t="n">
         <v>0.2442748091603053</v>
       </c>
-      <c r="E271" t="n">
-        <v>0.2580645161290323</v>
-      </c>
-      <c r="F271" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="272">
       <c r="A272" t="n">
@@ -5878,12 +4248,6 @@
       <c r="D272" t="n">
         <v>0.5572519083969466</v>
       </c>
-      <c r="E272" t="n">
-        <v>0.1290322580645161</v>
-      </c>
-      <c r="F272" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="273">
       <c r="A273" t="n">
@@ -5898,12 +4262,6 @@
       <c r="D273" t="n">
         <v>0.5648854961832062</v>
       </c>
-      <c r="E273" t="n">
-        <v>0.4193548387096774</v>
-      </c>
-      <c r="F273" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="274">
       <c r="A274" t="n">
@@ -5918,12 +4276,6 @@
       <c r="D274" t="n">
         <v>0</v>
       </c>
-      <c r="E274" t="n">
-        <v>0.1612903225806452</v>
-      </c>
-      <c r="F274" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="275">
       <c r="A275" t="n">
@@ -5938,12 +4290,6 @@
       <c r="D275" t="n">
         <v>0.648854961832061</v>
       </c>
-      <c r="E275" t="n">
-        <v>0.01612903225806452</v>
-      </c>
-      <c r="F275" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="276">
       <c r="A276" t="n">
@@ -5958,12 +4304,6 @@
       <c r="D276" t="n">
         <v>0.3587786259541985</v>
       </c>
-      <c r="E276" t="n">
-        <v>0.1612903225806452</v>
-      </c>
-      <c r="F276" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="277">
       <c r="A277" t="n">
@@ -5978,12 +4318,6 @@
       <c r="D277" t="n">
         <v>0.7404580152671756</v>
       </c>
-      <c r="E277" t="n">
-        <v>0.1612903225806452</v>
-      </c>
-      <c r="F277" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="278">
       <c r="A278" t="n">
@@ -5998,12 +4332,6 @@
       <c r="D278" t="n">
         <v>0.2595419847328244</v>
       </c>
-      <c r="E278" t="n">
-        <v>0.3225806451612903</v>
-      </c>
-      <c r="F278" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="279">
       <c r="A279" t="n">
@@ -6018,12 +4346,6 @@
       <c r="D279" t="n">
         <v>0.5343511450381679</v>
       </c>
-      <c r="E279" t="n">
-        <v>0.04838709677419355</v>
-      </c>
-      <c r="F279" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="280">
       <c r="A280" t="n">
@@ -6038,12 +4360,6 @@
       <c r="D280" t="n">
         <v>0.6183206106870229</v>
       </c>
-      <c r="E280" t="n">
-        <v>0</v>
-      </c>
-      <c r="F280" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="281">
       <c r="A281" t="n">
@@ -6058,12 +4374,6 @@
       <c r="D281" t="n">
         <v>0.4122137404580153</v>
       </c>
-      <c r="E281" t="n">
-        <v>0.5806451612903226</v>
-      </c>
-      <c r="F281" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="282">
       <c r="A282" t="n">
@@ -6078,12 +4388,6 @@
       <c r="D282" t="n">
         <v>0.4122137404580153</v>
       </c>
-      <c r="E282" t="n">
-        <v>0.2903225806451613</v>
-      </c>
-      <c r="F282" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="283">
       <c r="A283" t="n">
@@ -6098,12 +4402,6 @@
       <c r="D283" t="n">
         <v>0.648854961832061</v>
       </c>
-      <c r="E283" t="n">
-        <v>0.1612903225806452</v>
-      </c>
-      <c r="F283" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="284">
       <c r="A284" t="n">
@@ -6118,12 +4416,6 @@
       <c r="D284" t="n">
         <v>0.4809160305343512</v>
       </c>
-      <c r="E284" t="n">
-        <v>0.3548387096774194</v>
-      </c>
-      <c r="F284" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="285">
       <c r="A285" t="n">
@@ -6138,12 +4430,6 @@
       <c r="D285" t="n">
         <v>0.8396946564885496</v>
       </c>
-      <c r="E285" t="n">
-        <v>0</v>
-      </c>
-      <c r="F285" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="286">
       <c r="A286" t="n">
@@ -6158,12 +4444,6 @@
       <c r="D286" t="n">
         <v>0.5114503816793893</v>
       </c>
-      <c r="E286" t="n">
-        <v>0.3064516129032258</v>
-      </c>
-      <c r="F286" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
@@ -6178,12 +4458,6 @@
       <c r="D287" t="n">
         <v>0.3740458015267176</v>
       </c>
-      <c r="E287" t="n">
-        <v>0.2903225806451613</v>
-      </c>
-      <c r="F287" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
@@ -6198,12 +4472,6 @@
       <c r="D288" t="n">
         <v>0.6946564885496184</v>
       </c>
-      <c r="E288" t="n">
-        <v>0.1290322580645161</v>
-      </c>
-      <c r="F288" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="289">
       <c r="A289" t="n">
@@ -6218,12 +4486,6 @@
       <c r="D289" t="n">
         <v>0.7099236641221374</v>
       </c>
-      <c r="E289" t="n">
-        <v>0</v>
-      </c>
-      <c r="F289" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="290">
       <c r="A290" t="n">
@@ -6238,12 +4500,6 @@
       <c r="D290" t="n">
         <v>0.5496183206106871</v>
       </c>
-      <c r="E290" t="n">
-        <v>0.4838709677419354</v>
-      </c>
-      <c r="F290" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="291">
       <c r="A291" t="n">
@@ -6258,12 +4514,6 @@
       <c r="D291" t="n">
         <v>0.4503816793893129</v>
       </c>
-      <c r="E291" t="n">
-        <v>0.3225806451612903</v>
-      </c>
-      <c r="F291" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="292">
       <c r="A292" t="n">
@@ -6278,12 +4528,6 @@
       <c r="D292" t="n">
         <v>0.6870229007633588</v>
       </c>
-      <c r="E292" t="n">
-        <v>0</v>
-      </c>
-      <c r="F292" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="293">
       <c r="A293" t="n">
@@ -6298,12 +4542,6 @@
       <c r="D293" t="n">
         <v>0.5267175572519084</v>
       </c>
-      <c r="E293" t="n">
-        <v>0.7096774193548387</v>
-      </c>
-      <c r="F293" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="294">
       <c r="A294" t="n">
@@ -6318,12 +4556,6 @@
       <c r="D294" t="n">
         <v>0.5725190839694656</v>
       </c>
-      <c r="E294" t="n">
-        <v>0.4516129032258064</v>
-      </c>
-      <c r="F294" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="295">
       <c r="A295" t="n">
@@ -6338,12 +4570,6 @@
       <c r="D295" t="n">
         <v>0.6030534351145038</v>
       </c>
-      <c r="E295" t="n">
-        <v>0.1290322580645161</v>
-      </c>
-      <c r="F295" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
@@ -6358,12 +4584,6 @@
       <c r="D296" t="n">
         <v>0.5572519083969466</v>
       </c>
-      <c r="E296" t="n">
-        <v>0.4516129032258064</v>
-      </c>
-      <c r="F296" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="297">
       <c r="A297" t="n">
@@ -6378,12 +4598,6 @@
       <c r="D297" t="n">
         <v>0.5572519083969466</v>
       </c>
-      <c r="E297" t="n">
-        <v>0.6451612903225806</v>
-      </c>
-      <c r="F297" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="298">
       <c r="A298" t="n">
@@ -6398,12 +4612,6 @@
       <c r="D298" t="n">
         <v>0.4961832061068702</v>
       </c>
-      <c r="E298" t="n">
-        <v>0</v>
-      </c>
-      <c r="F298" t="n">
-        <v>0.6666666666666666</v>
-      </c>
     </row>
     <row r="299">
       <c r="A299" t="n">
@@ -6418,12 +4626,6 @@
       <c r="D299" t="n">
         <v>0.1450381679389313</v>
       </c>
-      <c r="E299" t="n">
-        <v>0.1612903225806452</v>
-      </c>
-      <c r="F299" t="n">
-        <v>0.3333333333333333</v>
-      </c>
     </row>
     <row r="300">
       <c r="A300" t="n">
@@ -6438,12 +4640,6 @@
       <c r="D300" t="n">
         <v>0.3969465648854962</v>
       </c>
-      <c r="E300" t="n">
-        <v>0.03225806451612903</v>
-      </c>
-      <c r="F300" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
@@ -6458,12 +4654,6 @@
       <c r="D301" t="n">
         <v>0.4656488549618321</v>
       </c>
-      <c r="E301" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F301" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="302">
       <c r="A302" t="n">
@@ -6478,12 +4668,6 @@
       <c r="D302" t="n">
         <v>0.5343511450381679</v>
       </c>
-      <c r="E302" t="n">
-        <v>0.5483870967741935</v>
-      </c>
-      <c r="F302" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="303">
       <c r="A303" t="n">
@@ -6498,12 +4682,6 @@
       <c r="D303" t="n">
         <v>0.3358778625954199</v>
       </c>
-      <c r="E303" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="F303" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="304">
       <c r="A304" t="n">
@@ -6517,12 +4695,6 @@
       </c>
       <c r="D304" t="n">
         <v>0.7862595419847328</v>
-      </c>
-      <c r="E304" t="n">
-        <v>0</v>
-      </c>
-      <c r="F304" t="n">
-        <v>0.6666666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>